<commit_message>
proving current matrix and RGF. Work on coeff
</commit_message>
<xml_diff>
--- a/src/RGF_input_file.xlsx
+++ b/src/RGF_input_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workshop\RGF\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AgVer\git\RGF\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Item</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -129,7 +129,19 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>BLG</t>
+    <t>Plot band structure</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Define GPU enable and max calculated matrix size</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MLG</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU max matrix</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1054,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1080,174 +1092,138 @@
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="b">
-        <v>0</v>
+      <c r="B2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <f>MAX(E12:E33)+1+IF(PRODUCT(C12:C33)&gt;1,1,0)</f>
-        <v>101</v>
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <f>SUM(F12:F34)</f>
-        <v>900</v>
+        <f>MAX(E14:E35)+1+IF(PRODUCT(C14:C35)&gt;1,1,0)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <f>SUM(F14:F36)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>100</v>
-      </c>
-      <c r="F12">
-        <v>300</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>2.5</v>
-      </c>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <v>300</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1262,7 +1238,7 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>300</v>
+        <v>10</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1271,13 +1247,71 @@
         <v>0</v>
       </c>
       <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="G12:I12"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
debugging T+R /= 1
</commit_message>
<xml_diff>
--- a/src/RGF_input_file.xlsx
+++ b/src/RGF_input_file.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Item</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -90,10 +90,6 @@
   </si>
   <si>
     <t>Using GPU</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1069,7 +1065,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1099,12 +1095,12 @@
         <v>4000</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1">
         <v>1000</v>
@@ -1123,7 +1119,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1140,7 +1136,7 @@
       </c>
       <c r="B7">
         <f>MAX(E14:E35)+1+IF(PRODUCT(C14:C35)&gt;1,1,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1149,7 +1145,7 @@
       </c>
       <c r="B8">
         <f>SUM(F14:F36)</f>
-        <v>10</v>
+        <v>900</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1165,7 +1161,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="b">
         <v>1</v>
@@ -1176,37 +1172,37 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
         <v>19</v>
-      </c>
-      <c r="E13" t="s">
-        <v>20</v>
       </c>
       <c r="F13" t="s">
         <v>15</v>
@@ -1235,10 +1231,10 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14">
-        <v>10</v>
+        <v>300</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1247,12 +1243,12 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1264,10 +1260,10 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1276,12 +1272,12 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1293,10 +1289,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1305,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add GPU support (debuggin)
</commit_message>
<xml_diff>
--- a/src/RGF_input_file.xlsx
+++ b/src/RGF_input_file.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Item</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -146,6 +146,14 @@
   </si>
   <si>
     <t>x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Width(nm)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Length(nm)</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1070,18 +1078,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="17.08984375" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1092,7 +1101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1106,7 +1115,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1114,7 +1123,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1122,7 +1131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1130,7 +1139,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1138,25 +1147,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <f>MAX(E14:E35)+1+IF(PRODUCT(C14:C35)&gt;1,1,0)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8">
         <f>SUM(F14:F36)</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1167,15 +1176,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1183,7 +1192,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
@@ -1195,8 +1204,14 @@
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1225,7 +1240,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1239,10 +1254,10 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F14">
-        <v>300</v>
+        <v>808</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1253,8 +1268,16 @@
       <c r="I14">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J14">
+        <f>E14*0.246*3^0.5/2</f>
+        <v>2.1304224933097191</v>
+      </c>
+      <c r="K14">
+        <f>F14*0.246*3</f>
+        <v>596.30399999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1283,7 +1306,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
debugging GPU != CPU
</commit_message>
<xml_diff>
--- a/src/RGF_input_file.xlsx
+++ b/src/RGF_input_file.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7280"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16820" windowHeight="7280"/>
   </bookViews>
   <sheets>
     <sheet name="__setup__" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t>Item</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -145,15 +145,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>Width(nm)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Length(nm)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>x</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Width(nm)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Length(nm)</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1081,7 +1081,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -1106,7 +1106,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>4000</v>
@@ -1162,7 +1162,7 @@
       </c>
       <c r="B8">
         <f>SUM(F14:F36)</f>
-        <v>808</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
@@ -1170,7 +1170,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
@@ -1181,7 +1181,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
@@ -1205,10 +1205,10 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" t="s">
         <v>32</v>
-      </c>
-      <c r="K12" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">
@@ -1257,7 +1257,7 @@
         <v>10</v>
       </c>
       <c r="F14">
-        <v>808</v>
+        <v>1000</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1266,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="J14">
         <f>E14*0.246*3^0.5/2</f>
@@ -1274,12 +1274,12 @@
       </c>
       <c r="K14">
         <f>F14*0.246*3</f>
-        <v>596.30399999999997</v>
+        <v>738</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1303,12 +1303,20 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0.05</v>
+        <v>0.1</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ref="J15:J16" si="0">E15*0.246*3^0.5/2</f>
+        <v>0.21304224933097188</v>
+      </c>
+      <c r="K15">
+        <f t="shared" ref="K15:K16" si="1">F15*0.246*3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1320,7 +1328,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1332,7 +1340,15 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0.05</v>
+        <v>0.1</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix BLG band bugs & add time monitor
</commit_message>
<xml_diff>
--- a/src/RGF_input_file.xlsx
+++ b/src/RGF_input_file.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Item</t>
   </si>
@@ -108,13 +108,42 @@
     <t>Gap Open (eV)</t>
   </si>
   <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Width(# of sub unit cell)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bottom Barrier</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top Barrier</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ribbon profile</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top Barrier (nm)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bottom Barrier (nm)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>o</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Width(# of sub unit cell)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>first boolean for enabling plot function. Second boolean for also plotting zoom in figures</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -712,7 +741,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -726,6 +755,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1049,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1060,9 +1092,10 @@
     <col min="1" max="1" width="17.125" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="4"/>
+    <col min="11" max="11" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1078,9 +1111,8 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1098,9 +1130,8 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1114,9 +1145,8 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1130,14 +1160,13 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1146,9 +1175,8 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1162,31 +1190,32 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2">
-        <f>MAX(E14:E74)+1+IF(MAX(C14:C74)=2,1,0)</f>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="4">
+        <f>MAX(E14:E114)+MAX(J14:J114)+MAX(L14:L114)+1+IF(MAX(C14:C74)=2,1,0)</f>
+        <v>116</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2">
-        <v>1000</v>
+        <f>SUM(F14:F33)</f>
+        <v>1807</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1195,9 +1224,8 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1213,25 +1241,27 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1245,9 +1275,8 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1" t="s">
@@ -1261,14 +1290,22 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="J12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -1282,7 +1319,7 @@
         <v>24</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>25</v>
@@ -1296,12 +1333,35 @@
       <c r="I13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="J13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
@@ -1313,32 +1373,52 @@
         <v>0</v>
       </c>
       <c r="E14" s="2">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F14" s="2">
-        <v>1000</v>
+        <v>807</v>
       </c>
       <c r="G14" s="2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H14" s="2">
         <v>0</v>
       </c>
       <c r="I14" s="2">
-        <v>1</v>
-      </c>
-      <c r="J14" s="4">
-        <f>E14*0.246*3^0.5/2</f>
-        <v>3.1956337399645784</v>
+        <v>0.1</v>
+      </c>
+      <c r="J14">
+        <v>46</v>
       </c>
       <c r="K14" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="L14" s="4">
+        <v>46</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="N14" s="4">
+        <f>(E14+C14-1)*0.246*3^0.5/2</f>
+        <v>4.899971734612353</v>
+      </c>
+      <c r="O14" s="4">
+        <f>(J14+C14-1)*0.246*3^0.5/2</f>
+        <v>9.799943469224706</v>
+      </c>
+      <c r="P14" s="4">
+        <f>(L14+C14-1)*0.246*3^0.5/2</f>
+        <v>9.799943469224706</v>
+      </c>
+      <c r="Q14" s="4">
         <f>F14*0.246*3</f>
-        <v>738</v>
+        <v>595.56600000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
@@ -1350,10 +1430,10 @@
         <v>0</v>
       </c>
       <c r="E15" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F15" s="2">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="G15" s="2">
         <v>0</v>
@@ -1365,15 +1445,37 @@
         <v>0</v>
       </c>
       <c r="J15" s="4">
-        <v>0.21304224933097188</v>
+        <v>0</v>
       </c>
       <c r="K15" s="4">
-        <v>0</v>
+        <v>0.4</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="N15" s="4">
+        <f t="shared" ref="N15:N16" si="0">(E15+C15-1)*0.246*3^0.5/2</f>
+        <v>4.2608449866194382</v>
+      </c>
+      <c r="O15" s="4">
+        <f t="shared" ref="O15:O16" si="1">(J15+C15-1)*0.246*3^0.5/2</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="4">
+        <f t="shared" ref="P15:P16" si="2">(L15+C15-1)*0.246*3^0.5/2</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="4">
+        <f t="shared" ref="Q15:Q16" si="3">F15*0.246*3</f>
+        <v>738</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
@@ -1400,16 +1502,41 @@
         <v>0</v>
       </c>
       <c r="J16" s="4">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="K16" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="L16" s="4">
+        <v>46</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="N16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="4">
+        <f t="shared" si="1"/>
+        <v>9.799943469224706</v>
+      </c>
+      <c r="P16" s="4">
+        <f t="shared" si="2"/>
+        <v>9.799943469224706</v>
+      </c>
+      <c r="Q16" s="4">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="N12:Q12"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J12:K12"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
revise band structure output
</commit_message>
<xml_diff>
--- a/src/RGF_input_file.xlsx
+++ b/src/RGF_input_file.xlsx
@@ -1,32 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\03_Program\RGF\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workshop\RGF_github\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88F1920-09A6-4845-AD68-13781F8DAFA8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7275"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="__setup__" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Item</t>
   </si>
   <si>
-    <t>Input</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -52,12 +50,6 @@
   </si>
   <si>
     <t>Armchair</t>
-  </si>
-  <si>
-    <t>Max ribbon width</t>
-  </si>
-  <si>
-    <t>Max ribbon length</t>
   </si>
   <si>
     <t>Bias(V)</t>
@@ -148,13 +140,29 @@
   </si>
   <si>
     <t>BLG</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mesh</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>first column for max sub cell number been calculated. Second column for kx sweep meshing</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -745,20 +753,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1080,463 +1088,450 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.125" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" style="4"/>
-    <col min="11" max="11" width="9" style="4"/>
+    <col min="9" max="9" width="9" style="3"/>
+    <col min="11" max="11" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>4000</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>4000</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
         <v>1000</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="4">
         <v>21</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="4">
-        <f>MAX(E14:E114)+MAX(J14:J114)+MAX(L14:L114)+1+IF(MAX(C14:C74)=2,1,0)</f>
-        <v>116</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="C7" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
+      <c r="A8" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B8" s="2">
-        <f>SUM(F14:F33)</f>
-        <v>1807</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="J8" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="C9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" t="s">
+        <v>31</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
         <v>23</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13" t="s">
-        <v>34</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R13" s="2"/>
+      <c r="F13" s="1">
+        <v>807</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J13">
+        <v>46</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="L13" s="3">
+        <v>46</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="N13" s="3">
+        <f>(E13+C13-1)*0.246*3^0.5/2</f>
+        <v>4.899971734612353</v>
+      </c>
+      <c r="O13" s="3">
+        <f>(J13+C13-1)*0.246*3^0.5/2</f>
+        <v>9.799943469224706</v>
+      </c>
+      <c r="P13" s="3">
+        <f>(L13+C13-1)*0.246*3^0.5/2</f>
+        <v>9.799943469224706</v>
+      </c>
+      <c r="Q13" s="3">
+        <f>F13*0.246*3</f>
+        <v>595.56600000000003</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>23</v>
-      </c>
-      <c r="F14" s="2">
-        <v>807</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="J14">
-        <v>46</v>
-      </c>
-      <c r="K14" s="4">
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>20</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
         <v>0.4</v>
       </c>
-      <c r="L14" s="4">
-        <v>46</v>
-      </c>
-      <c r="M14" s="4">
+      <c r="L14" s="3">
+        <v>0</v>
+      </c>
+      <c r="M14" s="3">
         <v>0.4</v>
       </c>
-      <c r="N14" s="4">
-        <f>(E14+C14-1)*0.246*3^0.5/2</f>
-        <v>4.899971734612353</v>
-      </c>
-      <c r="O14" s="4">
-        <f>(J14+C14-1)*0.246*3^0.5/2</f>
-        <v>9.799943469224706</v>
-      </c>
-      <c r="P14" s="4">
-        <f>(L14+C14-1)*0.246*3^0.5/2</f>
-        <v>9.799943469224706</v>
-      </c>
-      <c r="Q14" s="4">
-        <f>F14*0.246*3</f>
-        <v>595.56600000000003</v>
+      <c r="N14" s="3">
+        <f t="shared" ref="N14:N15" si="0">(E14+C14-1)*0.246*3^0.5/2</f>
+        <v>4.2608449866194382</v>
+      </c>
+      <c r="O14" s="3">
+        <f t="shared" ref="O14:O15" si="1">(J14+C14-1)*0.246*3^0.5/2</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="3">
+        <f t="shared" ref="P14:P15" si="2">(L14+C14-1)*0.246*3^0.5/2</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="3">
+        <f t="shared" ref="Q14:Q15" si="3">F14*0.246*3</f>
+        <v>738</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="2">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>20</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1000</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2">
-        <v>0</v>
-      </c>
-      <c r="J15" s="4">
-        <v>0</v>
-      </c>
-      <c r="K15" s="4">
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>46</v>
+      </c>
+      <c r="K15" s="3">
         <v>0.4</v>
       </c>
-      <c r="L15" s="4">
-        <v>0</v>
-      </c>
-      <c r="M15" s="4">
+      <c r="L15" s="3">
+        <v>46</v>
+      </c>
+      <c r="M15" s="3">
         <v>0.4</v>
       </c>
-      <c r="N15" s="4">
-        <f t="shared" ref="N15:N16" si="0">(E15+C15-1)*0.246*3^0.5/2</f>
-        <v>4.2608449866194382</v>
-      </c>
-      <c r="O15" s="4">
-        <f t="shared" ref="O15:O16" si="1">(J15+C15-1)*0.246*3^0.5/2</f>
-        <v>0</v>
-      </c>
-      <c r="P15" s="4">
-        <f t="shared" ref="P15:P16" si="2">(L15+C15-1)*0.246*3^0.5/2</f>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="4">
-        <f t="shared" ref="Q15:Q16" si="3">F15*0.246*3</f>
-        <v>738</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
-        <v>46</v>
-      </c>
-      <c r="K16" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="L16" s="4">
-        <v>46</v>
-      </c>
-      <c r="M16" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="N16" s="4">
+      <c r="N15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O16" s="4">
+      <c r="O15" s="3">
         <f t="shared" si="1"/>
         <v>9.799943469224706</v>
       </c>
-      <c r="P16" s="4">
+      <c r="P15" s="3">
         <f t="shared" si="2"/>
         <v>9.799943469224706</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="Q15" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:K11"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
debugging RGF. GPU inv has issue.
</commit_message>
<xml_diff>
--- a/src/RGF_input_file.xlsx
+++ b/src/RGF_input_file.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7280"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16830" windowHeight="9240"/>
   </bookViews>
   <sheets>
     <sheet name="__setup__" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Item</t>
   </si>
   <si>
-    <t>Input</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -52,12 +49,6 @@
   </si>
   <si>
     <t>Armchair</t>
-  </si>
-  <si>
-    <t>Max ribbon width</t>
-  </si>
-  <si>
-    <t>Max ribbon length</t>
   </si>
   <si>
     <t>Bias(V)</t>
@@ -139,15 +130,31 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>mesh</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>first column for max sub cell number been calculated. Second column for kx sweep meshing</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>MLG</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>x</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>o</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1081,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -1100,11 +1107,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1114,16 +1123,16 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2">
         <v>4000</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1133,7 +1142,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>1000</v>
@@ -1148,10 +1157,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1163,10 +1172,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1178,10 +1187,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1193,13 +1202,17 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3">
-        <f>MAX(E14:E114)+MAX(J14:J114)+MAX(L14:L114)+1+IF(MAX(C14:C74)=2,1,0)</f>
-        <v>116</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="B7" s="4">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1208,13 +1221,14 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1">
-        <f>SUM(F14:F33)</f>
-        <v>1807</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1224,15 +1238,17 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1"/>
+      <c r="C9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1241,17 +1257,13 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1259,163 +1271,205 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="5" t="s">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" t="s">
+        <v>31</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
+      <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
         <v>23</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13" t="s">
-        <v>34</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R13" s="1"/>
+      <c r="F13" s="1">
+        <v>807</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J13">
+        <v>46</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="L13" s="3">
+        <v>46</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="N13" s="3">
+        <f>(E13+C13-1)*0.246*3^0.5/2</f>
+        <v>4.899971734612353</v>
+      </c>
+      <c r="O13" s="3">
+        <f>(J13+C13-1)*0.246*3^0.5/2</f>
+        <v>9.799943469224706</v>
+      </c>
+      <c r="P13" s="3">
+        <f>(L13+C13-1)*0.246*3^0.5/2</f>
+        <v>9.799943469224706</v>
+      </c>
+      <c r="Q13" s="3">
+        <f>F13*0.246*3</f>
+        <v>595.56600000000003</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F14" s="1">
-        <v>807</v>
+        <v>500</v>
       </c>
       <c r="G14" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
       </c>
       <c r="I14" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="J14">
-        <v>46</v>
+        <v>0.25</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
       </c>
       <c r="K14" s="3">
         <v>0.4</v>
       </c>
       <c r="L14" s="3">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="M14" s="3">
         <v>0.4</v>
       </c>
       <c r="N14" s="3">
-        <f>(E14+C14-1)*0.246*3^0.5/2</f>
-        <v>4.899971734612353</v>
+        <f t="shared" ref="N14:N15" si="0">(E14+C14-1)*0.246*3^0.5/2</f>
+        <v>2.3434647426406907</v>
       </c>
       <c r="O14" s="3">
-        <f>(J14+C14-1)*0.246*3^0.5/2</f>
-        <v>9.799943469224706</v>
+        <f t="shared" ref="O14:O15" si="1">(J14+C14-1)*0.246*3^0.5/2</f>
+        <v>0.21304224933097188</v>
       </c>
       <c r="P14" s="3">
-        <f>(L14+C14-1)*0.246*3^0.5/2</f>
-        <v>9.799943469224706</v>
+        <f t="shared" ref="P14:P15" si="2">(L14+C14-1)*0.246*3^0.5/2</f>
+        <v>0.21304224933097188</v>
       </c>
       <c r="Q14" s="3">
-        <f>F14*0.246*3</f>
-        <v>595.56600000000003</v>
+        <f t="shared" ref="Q14:Q15" si="3">F14*0.246*3</f>
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -1427,10 +1481,10 @@
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
@@ -1442,98 +1496,41 @@
         <v>0</v>
       </c>
       <c r="J15" s="3">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="K15" s="3">
         <v>0.4</v>
       </c>
       <c r="L15" s="3">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="M15" s="3">
         <v>0.4</v>
       </c>
       <c r="N15" s="3">
-        <f t="shared" ref="N15:N16" si="0">(E15+C15-1)*0.246*3^0.5/2</f>
-        <v>4.2608449866194382</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="O15" s="3">
-        <f t="shared" ref="O15:O16" si="1">(J15+C15-1)*0.246*3^0.5/2</f>
-        <v>0</v>
-      </c>
-      <c r="P15" s="3">
-        <f t="shared" ref="P15:P16" si="2">(L15+C15-1)*0.246*3^0.5/2</f>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="3">
-        <f t="shared" ref="Q15:Q16" si="3">F15*0.246*3</f>
-        <v>738</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
-      <c r="J16" s="3">
-        <v>46</v>
-      </c>
-      <c r="K16" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="L16" s="3">
-        <v>46</v>
-      </c>
-      <c r="M16" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="N16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="3">
         <f t="shared" si="1"/>
         <v>9.799943469224706</v>
       </c>
-      <c r="P16" s="3">
+      <c r="P15" s="3">
         <f t="shared" si="2"/>
         <v>9.799943469224706</v>
       </c>
-      <c r="Q16" s="3">
+      <c r="Q15" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:K11"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
replace complex inv with scikit-cuda zgetrf
</commit_message>
<xml_diff>
--- a/src/RGF_input_file.xlsx
+++ b/src/RGF_input_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workshop\RGF\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\03_Program\RGF\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
   <si>
     <t>Item</t>
   </si>
@@ -155,6 +155,10 @@
   </si>
   <si>
     <t>o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1091,18 +1095,18 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.08984375" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.125" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="3"/>
     <col min="11" max="11" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1121,12 +1125,12 @@
       <c r="H1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2">
         <v>4000</v>
@@ -1140,7 +1144,7 @@
       <c r="H2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1155,7 +1159,7 @@
       <c r="H3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1170,7 +1174,7 @@
       <c r="H4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1185,7 +1189,7 @@
       <c r="H5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1200,7 +1204,7 @@
       <c r="H6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -1219,7 +1223,7 @@
       <c r="H7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1236,7 +1240,7 @@
       <c r="H8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1255,7 +1259,7 @@
       <c r="H9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1270,7 +1274,7 @@
       <c r="H10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="5" t="s">
@@ -1299,7 +1303,7 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1353,7 +1357,7 @@
       </c>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -1410,7 +1414,7 @@
         <v>595.56600000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
@@ -1467,7 +1471,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
add R_matrix support. Debug T and R matrix.
</commit_message>
<xml_diff>
--- a/src/RGF_input_file.xlsx
+++ b/src/RGF_input_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\03_Program\RGF\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workshop\github\RGF\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Item</t>
   </si>
@@ -155,10 +155,6 @@
   </si>
   <si>
     <t>o</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>T</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1095,18 +1091,18 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.125" customWidth="1"/>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.08984375" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="3"/>
     <col min="11" max="11" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1125,7 +1121,7 @@
       <c r="H1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1144,7 +1140,7 @@
       <c r="H2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1159,7 +1155,7 @@
       <c r="H3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1174,7 +1170,7 @@
       <c r="H4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1189,7 +1185,7 @@
       <c r="H5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1204,15 +1200,15 @@
       <c r="H6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="4">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C7" s="4">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>37</v>
@@ -1223,7 +1219,7 @@
       <c r="H7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1240,7 +1236,7 @@
       <c r="H8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1259,7 +1255,7 @@
       <c r="H9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1274,7 +1270,7 @@
       <c r="H10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="5" t="s">
@@ -1303,7 +1299,7 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1357,9 +1353,9 @@
       </c>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -1414,24 +1410,24 @@
         <v>595.56600000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F14" s="1">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
@@ -1440,7 +1436,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="1">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="J14" s="3">
         <v>0</v>
@@ -1456,22 +1452,22 @@
       </c>
       <c r="N14" s="3">
         <f t="shared" ref="N14:N15" si="0">(E14+C14-1)*0.246*3^0.5/2</f>
-        <v>0.42608449866194376</v>
+        <v>2.1304224933097191</v>
       </c>
       <c r="O14" s="3">
         <f t="shared" ref="O14:O15" si="1">(J14+C14-1)*0.246*3^0.5/2</f>
-        <v>0.21304224933097188</v>
+        <v>0</v>
       </c>
       <c r="P14" s="3">
         <f t="shared" ref="P14:P15" si="2">(L14+C14-1)*0.246*3^0.5/2</f>
-        <v>0.21304224933097188</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="3">
         <f t="shared" ref="Q14:Q15" si="3">F14*0.246*3</f>
-        <v>738</v>
+        <v>2.214</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>